<commit_message>
almost completed the compensation section. made a technological change in the UG, for the Ш8 bus, added a negative linear tolerance - 3 mm. to the side. and did the same so far with one side for the combined sections, for the Ш12 bus for side В
</commit_message>
<xml_diff>
--- a/Контрольная ведомость Заказ №195.xlsx
+++ b/Контрольная ведомость Заказ №195.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CR2-55-Al-2500-4-pt0.5</t>
+          <t>E3-55-Al-3200-4-zg</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -499,12 +499,12 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>прямая секция</t>
+          <t>z-образная горизонтальная</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>300*200*500</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -512,10 +512,8 @@
           <t>G-002</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I2" s="2" t="n">
+        <v>32</v>
       </c>
       <c r="J2" s="2" t="inlineStr"/>
     </row>
@@ -523,7 +521,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 195&amp;C&amp;"Century Gothic"&amp;20 Упаковка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_15 09 2021</oddHeader>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 195&amp;C&amp;"Century Gothic"&amp;20 Упаковка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_20 09 2021</oddHeader>
     <oddFooter>&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>

<commit_message>
correction of errors in the calculation of joints
</commit_message>
<xml_diff>
--- a/Контрольная ведомость Заказ №195.xlsx
+++ b/Контрольная ведомость Заказ №195.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>E3-55-Al-3200-4-zg</t>
+          <t>E3-55-Al-3200-4-sb</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -499,21 +499,17 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>z-образная горизонтальная</t>
+          <t>стыковочный блок</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>300*200*500</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>G-002</t>
-        </is>
-      </c>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="n">
-        <v>32</v>
+        <v>8.35</v>
       </c>
       <c r="J2" s="2" t="inlineStr"/>
     </row>
@@ -521,7 +517,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 195&amp;C&amp;"Century Gothic"&amp;20 Упаковка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_20 09 2021</oddHeader>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 195&amp;C&amp;"Century Gothic"&amp;20 Упаковка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_28 09 2021</oddHeader>
     <oddFooter>&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>